<commit_message>
Final - Main Spreadsheet w/charts
</commit_message>
<xml_diff>
--- a/Final_Capstone_Spreadsheet_wtih_charts.xlsx
+++ b/Final_Capstone_Spreadsheet_wtih_charts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\Northwest University\M.S. in Data Analytics\Data Analytics Capstone Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2179F254-C86A-4314-B612-8626DEAA047A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70857C54-46BB-49D4-871B-F86DCB872568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C84C568-BB1D-4E22-BFF7-82713F13B653}"/>
+    <workbookView xWindow="2250" yWindow="1050" windowWidth="20550" windowHeight="14550" xr2:uid="{5C84C568-BB1D-4E22-BFF7-82713F13B653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1616,7 +1616,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Final_Capstone_Spreadsheet2.xlsx]Suggestion2!PivotTable2</c:name>
+    <c:name>[Final_Capstone_Spreadsheet_wtih_charts.xlsx]Suggestion2!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1772,6 +1772,9 @@
           </a:ln>
           <a:effectLst/>
         </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:spPr>
@@ -1814,6 +1817,18 @@
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="ED7331"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -4711,7 +4726,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0313DF9-723E-41E7-BAC7-07EACE4EF570}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D0313DF9-723E-41E7-BAC7-07EACE4EF570}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A2:B31" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
@@ -4892,7 +4907,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F9DDF090-B391-4F8A-9B84-B27E12B64009}" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F9DDF090-B391-4F8A-9B84-B27E12B64009}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A2:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
@@ -5345,8 +5360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332728E2-40ED-4FF8-A63E-ACB59181D2D0}">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:T21"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6719,7 +6734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BD7759-6736-452F-B58B-28DFBBA22EB5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>

</xml_diff>